<commit_message>
Combined Statitstic Values for the rest of the Cameras
</commit_message>
<xml_diff>
--- a/Dokumente/Verhältnisse.xlsx
+++ b/Dokumente/Verhältnisse.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>mvk021</t>
   </si>
@@ -433,7 +433,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -463,7 +463,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -487,7 +487,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>2361</v>
@@ -505,10 +505,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>6747</v>
@@ -529,7 +529,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>631</v>
@@ -546,6 +546,12 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
       <c r="D6">
         <v>14234</v>
       </c>
@@ -586,7 +592,7 @@
         <v>0</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" ref="G8:G25" si="0">100/(D8+D9)*D8</f>
+        <f t="shared" ref="G8" si="0">100/(D8+D9)*D8</f>
         <v>95.291354434626996</v>
       </c>
     </row>
@@ -601,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" ref="G9:G25" si="1">100/(D8+D9)*D9</f>
+        <f t="shared" ref="G9" si="1">100/(D8+D9)*D9</f>
         <v>4.7086455653730006</v>
       </c>
     </row>
@@ -616,7 +622,7 @@
         <v>0</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" ref="G10:G25" si="2">100/(D10+D11)*D10</f>
+        <f t="shared" ref="G10" si="2">100/(D10+D11)*D10</f>
         <v>89.574166604519348</v>
       </c>
     </row>
@@ -631,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" ref="G11:G25" si="3">100/(D10+D11)*D11</f>
+        <f t="shared" ref="G11" si="3">100/(D10+D11)*D11</f>
         <v>10.425833395480646</v>
       </c>
     </row>
@@ -646,7 +652,7 @@
         <v>0</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" ref="G12:G25" si="4">100/(D12+D13)*D12</f>
+        <f t="shared" ref="G12" si="4">100/(D12+D13)*D12</f>
         <v>93.842389642165358</v>
       </c>
     </row>
@@ -661,7 +667,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" ref="G13:G25" si="5">100/(D12+D13)*D13</f>
+        <f t="shared" ref="G13" si="5">100/(D12+D13)*D13</f>
         <v>6.1576103578346411</v>
       </c>
     </row>
@@ -676,7 +682,7 @@
         <v>0</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" ref="G14:G25" si="6">100/(D14+D15)*D14</f>
+        <f t="shared" ref="G14" si="6">100/(D14+D15)*D14</f>
         <v>90.742841887472466</v>
       </c>
     </row>
@@ -691,7 +697,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" ref="G15:G25" si="7">100/(D14+D15)*D15</f>
+        <f t="shared" ref="G15" si="7">100/(D14+D15)*D15</f>
         <v>9.2571581125275308</v>
       </c>
     </row>
@@ -706,7 +712,7 @@
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <f t="shared" ref="G16:G25" si="8">100/(D16+D17)*D16</f>
+        <f t="shared" ref="G16" si="8">100/(D16+D17)*D16</f>
         <v>91.730490581660121</v>
       </c>
     </row>
@@ -721,7 +727,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="1">
-        <f t="shared" ref="G17:G25" si="9">100/(D16+D17)*D17</f>
+        <f t="shared" ref="G17" si="9">100/(D16+D17)*D17</f>
         <v>8.2695094183398883</v>
       </c>
     </row>
@@ -736,7 +742,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="1">
-        <f t="shared" ref="G18:G25" si="10">100/(D18+D19)*D18</f>
+        <f t="shared" ref="G18" si="10">100/(D18+D19)*D18</f>
         <v>60.591294377789602</v>
       </c>
     </row>
@@ -751,7 +757,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="1">
-        <f t="shared" ref="G19:G25" si="11">100/(D18+D19)*D19</f>
+        <f t="shared" ref="G19" si="11">100/(D18+D19)*D19</f>
         <v>39.408705622210391</v>
       </c>
     </row>
@@ -766,7 +772,7 @@
         <v>0</v>
       </c>
       <c r="G20" s="1">
-        <f t="shared" ref="G20:G25" si="12">100/(D20+D21)*D20</f>
+        <f t="shared" ref="G20" si="12">100/(D20+D21)*D20</f>
         <v>68.276371554103974</v>
       </c>
     </row>
@@ -781,7 +787,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1">
-        <f t="shared" ref="G21:G25" si="13">100/(D20+D21)*D21</f>
+        <f t="shared" ref="G21" si="13">100/(D20+D21)*D21</f>
         <v>31.723628445896029</v>
       </c>
     </row>
@@ -811,7 +817,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="1">
-        <f t="shared" ref="G23:G25" si="14">100/(D22+D23)*D23</f>
+        <f t="shared" ref="G23" si="14">100/(D22+D23)*D23</f>
         <v>12.713885286365727</v>
       </c>
     </row>
@@ -826,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="G24" s="1">
-        <f t="shared" ref="G24:G25" si="15">100/(D24+D25)*D24</f>
+        <f t="shared" ref="G24" si="15">100/(D24+D25)*D24</f>
         <v>60.978758850478968</v>
       </c>
     </row>

</xml_diff>